<commit_message>
commit all changes for write to excel files
</commit_message>
<xml_diff>
--- a/testResource/CMVC_Trends.xlsx
+++ b/testResource/CMVC_Trends.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="225" windowWidth="11775" windowHeight="3030" tabRatio="730"/>
+    <workbookView xWindow="240" yWindow="225" windowWidth="11775" windowHeight="3030" tabRatio="730" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Overall" sheetId="9" r:id="rId1"/>
@@ -977,8 +977,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="176" formatCode="yyyy/m/d;@"/>
+    <numFmt numFmtId="177" formatCode="0_ "/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -1043,7 +1044,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1063,6 +1064,8 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1107,7 +1110,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1477,11 +1479,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="46742912"/>
-        <c:axId val="46752896"/>
+        <c:axId val="180181632"/>
+        <c:axId val="180191616"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="46742912"/>
+        <c:axId val="180181632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1490,7 +1492,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="46752896"/>
+        <c:crossAx val="180191616"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1498,7 +1500,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="46752896"/>
+        <c:axId val="180191616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1509,14 +1511,13 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="46742912"/>
+        <c:crossAx val="180181632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1685,7 +1686,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2055,11 +2055,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="46721664"/>
-        <c:axId val="47059328"/>
+        <c:axId val="182040448"/>
+        <c:axId val="182041984"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="46721664"/>
+        <c:axId val="182040448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2068,7 +2068,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="47059328"/>
+        <c:crossAx val="182041984"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2076,7 +2076,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="47059328"/>
+        <c:axId val="182041984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2087,14 +2087,13 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="46721664"/>
+        <c:crossAx val="182040448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2144,7 +2143,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2514,11 +2512,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="47115648"/>
-        <c:axId val="47117440"/>
+        <c:axId val="182094464"/>
+        <c:axId val="182104448"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="47115648"/>
+        <c:axId val="182094464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2527,7 +2525,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="47117440"/>
+        <c:crossAx val="182104448"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2535,7 +2533,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="47117440"/>
+        <c:axId val="182104448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2546,14 +2544,13 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="47115648"/>
+        <c:crossAx val="182094464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2603,7 +2600,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2811,11 +2807,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="47216896"/>
-        <c:axId val="47222784"/>
+        <c:axId val="182150272"/>
+        <c:axId val="182151808"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="47216896"/>
+        <c:axId val="182150272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2824,7 +2820,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="47222784"/>
+        <c:crossAx val="182151808"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2832,7 +2828,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="47222784"/>
+        <c:axId val="182151808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2843,14 +2839,13 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="47216896"/>
+        <c:crossAx val="182150272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -3647,7 +3642,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N20" sqref="N20"/>
     </sheetView>
   </sheetViews>
@@ -6032,22 +6027,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H47"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A37" sqref="A37:XFD37"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="2" max="2" width="13.25" customWidth="1"/>
+    <col min="1" max="1" width="9" style="14"/>
+    <col min="2" max="2" width="13.25" style="3" customWidth="1"/>
     <col min="3" max="3" width="22.375" customWidth="1"/>
     <col min="4" max="4" width="19.875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="6" t="s">
         <v>21</v>
       </c>
       <c r="C1" s="2" t="s">
@@ -6061,7 +6057,7 @@
       <c r="H1" s="5"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A2">
+      <c r="A2" s="14">
         <v>192969</v>
       </c>
       <c r="B2" s="3">
@@ -6069,175 +6065,175 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A3">
-        <v>192992</v>
+      <c r="A3" s="14">
+        <v>193648</v>
       </c>
       <c r="B3" s="3">
-        <v>41415</v>
+        <v>41152</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A4">
-        <v>193648</v>
+      <c r="A4" s="14">
+        <v>194161</v>
       </c>
       <c r="B4" s="3">
-        <v>41152</v>
+        <v>41191</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A5">
-        <v>194161</v>
+      <c r="A5" s="14">
+        <v>195291</v>
       </c>
       <c r="B5" s="3">
-        <v>41191</v>
+        <v>41260</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A6">
-        <v>195291</v>
+      <c r="A6" s="14">
+        <v>195386</v>
       </c>
       <c r="B6" s="3">
-        <v>41260</v>
+        <v>41269</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A7">
-        <v>195386</v>
+      <c r="A7" s="14">
+        <v>195415</v>
       </c>
       <c r="B7" s="3">
         <v>41269</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A8">
-        <v>195415</v>
+      <c r="A8" s="14">
+        <v>195518</v>
       </c>
       <c r="B8" s="3">
-        <v>41269</v>
+        <v>41282</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A9">
-        <v>195518</v>
+      <c r="A9" s="14">
+        <v>195975</v>
       </c>
       <c r="B9" s="3">
-        <v>41282</v>
+        <v>41310</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A10">
-        <v>195975</v>
+      <c r="A10" s="14">
+        <v>195983</v>
       </c>
       <c r="B10" s="3">
         <v>41310</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A11">
-        <v>195983</v>
+      <c r="A11" s="14">
+        <v>195990</v>
       </c>
       <c r="B11" s="3">
         <v>41310</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A12">
-        <v>195990</v>
+      <c r="A12" s="14">
+        <v>195992</v>
       </c>
       <c r="B12" s="3">
         <v>41310</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A13">
-        <v>195992</v>
+      <c r="A13" s="14">
+        <v>196216</v>
       </c>
       <c r="B13" s="3">
-        <v>41310</v>
+        <v>41324</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A14">
-        <v>196216</v>
+      <c r="A14" s="14">
+        <v>196305</v>
       </c>
       <c r="B14" s="3">
-        <v>41324</v>
+        <v>41331</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A15">
-        <v>196305</v>
+      <c r="A15" s="14">
+        <v>196343</v>
       </c>
       <c r="B15" s="3">
-        <v>41331</v>
+        <v>41338</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A16">
-        <v>196328</v>
+      <c r="A16" s="14">
+        <v>196518</v>
       </c>
       <c r="B16" s="3">
-        <v>41352</v>
+        <v>41344</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A17">
-        <v>196343</v>
+      <c r="A17" s="14">
+        <v>196521</v>
       </c>
       <c r="B17" s="3">
-        <v>41338</v>
+        <v>41344</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A18">
-        <v>196518</v>
+      <c r="A18" s="14">
+        <v>196561</v>
       </c>
       <c r="B18" s="3">
         <v>41344</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A19">
-        <v>196521</v>
+      <c r="A19" s="14">
+        <v>196585</v>
       </c>
       <c r="B19" s="3">
         <v>41344</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A20">
-        <v>196561</v>
+      <c r="A20" s="14">
+        <v>196593</v>
       </c>
       <c r="B20" s="3">
         <v>41344</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A21">
-        <v>196585</v>
+      <c r="A21" s="14">
+        <v>196602</v>
       </c>
       <c r="B21" s="3">
         <v>41344</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A22">
-        <v>196593</v>
+      <c r="A22" s="14">
+        <v>196659</v>
       </c>
       <c r="B22" s="3">
-        <v>41344</v>
+        <v>41345</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A23">
-        <v>196602</v>
+      <c r="A23" s="14">
+        <v>196328</v>
       </c>
       <c r="B23" s="3">
-        <v>41344</v>
+        <v>41352</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A24">
+      <c r="A24" s="14">
         <v>196657</v>
       </c>
       <c r="B24" s="3">
@@ -6245,115 +6241,115 @@
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A25">
-        <v>196659</v>
+      <c r="A25" s="14">
+        <v>196816</v>
       </c>
       <c r="B25" s="3">
-        <v>41345</v>
+        <v>41358</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A26">
-        <v>196816</v>
+      <c r="A26" s="14">
+        <v>196841</v>
       </c>
       <c r="B26" s="3">
         <v>41358</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A27">
-        <v>196841</v>
+      <c r="A27" s="14">
+        <v>196954</v>
       </c>
       <c r="B27" s="3">
-        <v>41358</v>
+        <v>41366</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A28">
+      <c r="A28" s="14">
+        <v>196965</v>
+      </c>
+      <c r="B28" s="3">
+        <v>41366</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A29" s="14">
+        <v>197246</v>
+      </c>
+      <c r="B29" s="3">
+        <v>41387</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A30" s="14">
+        <v>197678</v>
+      </c>
+      <c r="B30" s="3">
+        <v>41401</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A31" s="14">
         <v>196872</v>
       </c>
-      <c r="B28" s="3">
+      <c r="B31" s="3">
         <v>41408</v>
       </c>
-      <c r="C28" s="3"/>
-      <c r="D28" t="s">
+      <c r="C31" s="3"/>
+      <c r="D31" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A29">
-        <v>196954</v>
-      </c>
-      <c r="B29" s="3">
-        <v>41366</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A30">
-        <v>196965</v>
-      </c>
-      <c r="B30" s="3">
-        <v>41366</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A31">
-        <v>197246</v>
-      </c>
-      <c r="B31" s="3">
-        <v>41387</v>
-      </c>
-    </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A32">
-        <v>197678</v>
+      <c r="A32" s="14">
+        <v>197880</v>
       </c>
       <c r="B32" s="3">
-        <v>41401</v>
+        <v>41408</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A33">
-        <v>197880</v>
+      <c r="A33" s="14">
+        <v>197927</v>
       </c>
       <c r="B33" s="3">
         <v>41408</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A34">
-        <v>197927</v>
+      <c r="A34" s="14">
+        <v>192992</v>
       </c>
       <c r="B34" s="3">
-        <v>41408</v>
+        <v>41415</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A35">
-        <v>197958</v>
+      <c r="A35" s="14">
+        <v>197975</v>
       </c>
       <c r="B35" s="3">
-        <v>41422</v>
+        <v>41415</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A36">
-        <v>197975</v>
+      <c r="A36" s="14">
+        <v>197997</v>
       </c>
       <c r="B36" s="3">
         <v>41415</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A37">
-        <v>197997</v>
+      <c r="A37" s="14">
+        <v>197958</v>
       </c>
       <c r="B37" s="3">
-        <v>41415</v>
+        <v>41422</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A38">
+      <c r="A38" s="14">
         <v>198116</v>
       </c>
       <c r="B38" s="3">
@@ -6361,7 +6357,7 @@
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A39">
+      <c r="A39" s="14">
         <v>198117</v>
       </c>
       <c r="B39" s="3">
@@ -6369,7 +6365,7 @@
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A40">
+      <c r="A40" s="14">
         <v>198130</v>
       </c>
       <c r="B40" s="3">
@@ -6377,7 +6373,7 @@
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A41">
+      <c r="A41" s="14">
         <v>198150</v>
       </c>
       <c r="B41" s="3">
@@ -6385,7 +6381,7 @@
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A42">
+      <c r="A42" s="14">
         <v>198151</v>
       </c>
       <c r="B42" s="3">
@@ -6393,7 +6389,7 @@
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A43">
+      <c r="A43" s="14">
         <v>198160</v>
       </c>
       <c r="B43" s="3">
@@ -6401,7 +6397,7 @@
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A44">
+      <c r="A44" s="14">
         <v>198179</v>
       </c>
       <c r="B44" s="3">
@@ -6409,7 +6405,7 @@
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A45">
+      <c r="A45" s="14">
         <v>198196</v>
       </c>
       <c r="B45" s="3">
@@ -6417,7 +6413,7 @@
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A46">
+      <c r="A46" s="14">
         <v>198237</v>
       </c>
       <c r="B46" s="3">
@@ -6425,7 +6421,7 @@
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A47">
+      <c r="A47" s="14">
         <v>198251</v>
       </c>
       <c r="B47" s="3">
@@ -6434,7 +6430,7 @@
     </row>
   </sheetData>
   <sortState ref="A2:D47">
-    <sortCondition ref="A10"/>
+    <sortCondition ref="B8"/>
   </sortState>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6446,17 +6442,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S329"/>
   <sheetViews>
-    <sheetView topLeftCell="A301" workbookViewId="0">
-      <selection activeCell="C320" sqref="C320"/>
+    <sheetView topLeftCell="A169" workbookViewId="0">
+      <selection activeCell="A169" sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
+    <col min="1" max="1" width="9" style="14"/>
     <col min="2" max="3" width="11.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="13" t="s">
         <v>19</v>
       </c>
       <c r="B1" s="2" t="s">
@@ -6467,7 +6464,7 @@
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="A2">
+      <c r="A2" s="14">
         <v>190340</v>
       </c>
       <c r="B2" s="3">
@@ -6478,7 +6475,7 @@
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="A3">
+      <c r="A3" s="14">
         <v>196889</v>
       </c>
       <c r="B3" s="3">
@@ -6489,7 +6486,7 @@
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="A4">
+      <c r="A4" s="14">
         <v>190435</v>
       </c>
       <c r="B4" s="3">
@@ -6500,7 +6497,7 @@
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="A5">
+      <c r="A5" s="14">
         <v>191062</v>
       </c>
       <c r="B5" s="3">
@@ -6511,7 +6508,7 @@
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="A6">
+      <c r="A6" s="14">
         <v>183311</v>
       </c>
       <c r="B6" s="3">
@@ -6522,7 +6519,7 @@
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="A7">
+      <c r="A7" s="14">
         <v>190619</v>
       </c>
       <c r="B7" s="3">
@@ -6536,7 +6533,7 @@
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="A8">
+      <c r="A8" s="14">
         <v>190620</v>
       </c>
       <c r="B8" s="3">
@@ -6577,7 +6574,7 @@
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="A9">
+      <c r="A9" s="14">
         <v>191292</v>
       </c>
       <c r="B9" s="3">
@@ -6618,7 +6615,7 @@
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="A10">
+      <c r="A10" s="14">
         <v>191375</v>
       </c>
       <c r="B10" s="3">
@@ -6659,7 +6656,7 @@
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="A11">
+      <c r="A11" s="14">
         <v>191174</v>
       </c>
       <c r="B11" s="3">
@@ -6700,7 +6697,7 @@
       </c>
     </row>
     <row r="12" spans="1:19" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12">
+      <c r="A12" s="14">
         <v>191425</v>
       </c>
       <c r="B12" s="3">
@@ -6714,7 +6711,7 @@
       <c r="H12" s="5"/>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="A13">
+      <c r="A13" s="14">
         <v>178979</v>
       </c>
       <c r="B13" s="4">
@@ -6725,7 +6722,7 @@
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="A14">
+      <c r="A14" s="14">
         <v>189981</v>
       </c>
       <c r="B14" s="3">
@@ -6736,7 +6733,7 @@
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="A15">
+      <c r="A15" s="14">
         <v>190797</v>
       </c>
       <c r="B15" s="3">
@@ -6747,7 +6744,7 @@
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="A16">
+      <c r="A16" s="14">
         <v>190495</v>
       </c>
       <c r="B16" s="3">
@@ -6758,7 +6755,7 @@
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A17">
+      <c r="A17" s="14">
         <v>191376</v>
       </c>
       <c r="B17" s="3">
@@ -6769,7 +6766,7 @@
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A18">
+      <c r="A18" s="14">
         <v>189997</v>
       </c>
       <c r="B18" s="3">
@@ -6780,7 +6777,7 @@
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A19">
+      <c r="A19" s="14">
         <v>190496</v>
       </c>
       <c r="B19" s="3">
@@ -6791,7 +6788,7 @@
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A20">
+      <c r="A20" s="14">
         <v>191789</v>
       </c>
       <c r="B20" s="3">
@@ -6802,7 +6799,7 @@
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A21">
+      <c r="A21" s="14">
         <v>190347</v>
       </c>
       <c r="B21" s="3">
@@ -6813,7 +6810,7 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A22">
+      <c r="A22" s="14">
         <v>191155</v>
       </c>
       <c r="B22" s="3">
@@ -6824,7 +6821,7 @@
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A23">
+      <c r="A23" s="14">
         <v>191273</v>
       </c>
       <c r="B23" s="3">
@@ -6835,7 +6832,7 @@
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A24">
+      <c r="A24" s="14">
         <v>191910</v>
       </c>
       <c r="B24" s="3">
@@ -6846,7 +6843,7 @@
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A25">
+      <c r="A25" s="14">
         <v>192037</v>
       </c>
       <c r="B25" s="3">
@@ -6860,7 +6857,7 @@
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A26">
+      <c r="A26" s="14">
         <v>191764</v>
       </c>
       <c r="B26" s="3">
@@ -6871,7 +6868,7 @@
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A27">
+      <c r="A27" s="14">
         <v>191767</v>
       </c>
       <c r="B27" s="3">
@@ -6882,7 +6879,7 @@
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A28">
+      <c r="A28" s="14">
         <v>191788</v>
       </c>
       <c r="B28" s="3">
@@ -6893,7 +6890,7 @@
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A29">
+      <c r="A29" s="14">
         <v>192431</v>
       </c>
       <c r="B29" s="3">
@@ -6904,7 +6901,7 @@
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A30">
+      <c r="A30" s="14">
         <v>192634</v>
       </c>
       <c r="B30" s="3">
@@ -6915,7 +6912,7 @@
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A31">
+      <c r="A31" s="14">
         <v>192652</v>
       </c>
       <c r="B31" s="3">
@@ -6926,7 +6923,7 @@
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A32">
+      <c r="A32" s="14">
         <v>190666</v>
       </c>
       <c r="B32" s="3">
@@ -6937,7 +6934,7 @@
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A33">
+      <c r="A33" s="14">
         <v>192690</v>
       </c>
       <c r="B33" s="3">
@@ -6948,7 +6945,7 @@
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A34">
+      <c r="A34" s="14">
         <v>192864</v>
       </c>
       <c r="B34" s="3">
@@ -6959,7 +6956,7 @@
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A35">
+      <c r="A35" s="14">
         <v>193076</v>
       </c>
       <c r="B35" s="3">
@@ -6970,7 +6967,7 @@
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A36">
+      <c r="A36" s="14">
         <v>193012</v>
       </c>
       <c r="B36" s="3">
@@ -6981,7 +6978,7 @@
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A37">
+      <c r="A37" s="14">
         <v>193075</v>
       </c>
       <c r="B37" s="3">
@@ -6992,7 +6989,7 @@
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A38">
+      <c r="A38" s="14">
         <v>192824</v>
       </c>
       <c r="B38" s="3">
@@ -7003,7 +7000,7 @@
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A39">
+      <c r="A39" s="14">
         <v>192809</v>
       </c>
       <c r="B39" s="3">
@@ -7014,7 +7011,7 @@
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A40">
+      <c r="A40" s="14">
         <v>193202</v>
       </c>
       <c r="B40" s="3">
@@ -7025,7 +7022,7 @@
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A41">
+      <c r="A41" s="14">
         <v>193241</v>
       </c>
       <c r="B41" s="3">
@@ -7036,7 +7033,7 @@
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A42">
+      <c r="A42" s="14">
         <v>193261</v>
       </c>
       <c r="B42" s="3">
@@ -7047,7 +7044,7 @@
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A43">
+      <c r="A43" s="14">
         <v>190407</v>
       </c>
       <c r="B43" s="3">
@@ -7058,7 +7055,7 @@
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A44">
+      <c r="A44" s="14">
         <v>192862</v>
       </c>
       <c r="B44" s="3">
@@ -7069,7 +7066,7 @@
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A45">
+      <c r="A45" s="14">
         <v>192961</v>
       </c>
       <c r="B45" s="3">
@@ -7080,7 +7077,7 @@
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A46">
+      <c r="A46" s="14">
         <v>193232</v>
       </c>
       <c r="B46" s="3">
@@ -7091,7 +7088,7 @@
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A47">
+      <c r="A47" s="14">
         <v>192839</v>
       </c>
       <c r="B47" s="3">
@@ -7102,7 +7099,7 @@
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A48">
+      <c r="A48" s="14">
         <v>193318</v>
       </c>
       <c r="B48" s="3">
@@ -7113,7 +7110,7 @@
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A49">
+      <c r="A49" s="14">
         <v>193330</v>
       </c>
       <c r="B49" s="3">
@@ -7124,7 +7121,7 @@
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A50">
+      <c r="A50" s="14">
         <v>193382</v>
       </c>
       <c r="B50" s="3">
@@ -7135,7 +7132,7 @@
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A51">
+      <c r="A51" s="14">
         <v>193383</v>
       </c>
       <c r="B51" s="3">
@@ -7146,7 +7143,7 @@
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A52">
+      <c r="A52" s="14">
         <v>193216</v>
       </c>
       <c r="B52" s="3">
@@ -7160,7 +7157,7 @@
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A53">
+      <c r="A53" s="14">
         <v>193367</v>
       </c>
       <c r="B53" s="3">
@@ -7171,7 +7168,7 @@
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A54">
+      <c r="A54" s="14">
         <v>190422</v>
       </c>
       <c r="B54" s="3">
@@ -7182,7 +7179,7 @@
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A55">
+      <c r="A55" s="14">
         <v>193302</v>
       </c>
       <c r="B55" s="3">
@@ -7193,7 +7190,7 @@
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A56">
+      <c r="A56" s="14">
         <v>193303</v>
       </c>
       <c r="B56" s="3">
@@ -7204,7 +7201,7 @@
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A57">
+      <c r="A57" s="14">
         <v>193384</v>
       </c>
       <c r="B57" s="3">
@@ -7215,7 +7212,7 @@
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A58">
+      <c r="A58" s="14">
         <v>193448</v>
       </c>
       <c r="B58" s="3">
@@ -7226,7 +7223,7 @@
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A59">
+      <c r="A59" s="14">
         <v>190300</v>
       </c>
       <c r="B59" s="3">
@@ -7237,7 +7234,7 @@
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A60">
+      <c r="A60" s="14">
         <v>193466</v>
       </c>
       <c r="B60" s="3">
@@ -7248,7 +7245,7 @@
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A61">
+      <c r="A61" s="14">
         <v>191406</v>
       </c>
       <c r="B61" s="3">
@@ -7259,7 +7256,7 @@
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A62">
+      <c r="A62" s="14">
         <v>192790</v>
       </c>
       <c r="B62" s="3">
@@ -7270,7 +7267,7 @@
       </c>
     </row>
     <row r="63" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A63">
+      <c r="A63" s="14">
         <v>192814</v>
       </c>
       <c r="B63" s="3">
@@ -7281,7 +7278,7 @@
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A64">
+      <c r="A64" s="14">
         <v>192892</v>
       </c>
       <c r="B64" s="3">
@@ -7292,7 +7289,7 @@
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A65">
+      <c r="A65" s="14">
         <v>193321</v>
       </c>
       <c r="B65" s="3">
@@ -7303,7 +7300,7 @@
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A66">
+      <c r="A66" s="14">
         <v>193336</v>
       </c>
       <c r="B66" s="3">
@@ -7314,7 +7311,7 @@
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A67">
+      <c r="A67" s="14">
         <v>193509</v>
       </c>
       <c r="B67" s="3">
@@ -7325,7 +7322,7 @@
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A68">
+      <c r="A68" s="14">
         <v>193180</v>
       </c>
       <c r="B68" s="3">
@@ -7336,7 +7333,7 @@
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A69">
+      <c r="A69" s="14">
         <v>193325</v>
       </c>
       <c r="B69" s="3">
@@ -7347,7 +7344,7 @@
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A70">
+      <c r="A70" s="14">
         <v>193327</v>
       </c>
       <c r="B70" s="3">
@@ -7358,7 +7355,7 @@
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A71">
+      <c r="A71" s="14">
         <v>193328</v>
       </c>
       <c r="B71" s="3">
@@ -7369,7 +7366,7 @@
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A72">
+      <c r="A72" s="14">
         <v>193470</v>
       </c>
       <c r="B72" s="3">
@@ -7380,7 +7377,7 @@
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A73">
+      <c r="A73" s="14">
         <v>193473</v>
       </c>
       <c r="B73" s="3">
@@ -7391,7 +7388,7 @@
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A74">
+      <c r="A74" s="14">
         <v>190719</v>
       </c>
       <c r="B74" s="3">
@@ -7402,7 +7399,7 @@
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A75">
+      <c r="A75" s="14">
         <v>193193</v>
       </c>
       <c r="B75" s="3">
@@ -7413,7 +7410,7 @@
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A76">
+      <c r="A76" s="14">
         <v>193474</v>
       </c>
       <c r="B76" s="3">
@@ -7424,7 +7421,7 @@
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A77">
+      <c r="A77" s="14">
         <v>193165</v>
       </c>
       <c r="B77" s="3">
@@ -7435,7 +7432,7 @@
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A78">
+      <c r="A78" s="14">
         <v>193416</v>
       </c>
       <c r="B78" s="3">
@@ -7446,7 +7443,7 @@
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A79">
+      <c r="A79" s="14">
         <v>193537</v>
       </c>
       <c r="B79" s="3">
@@ -7457,7 +7454,7 @@
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A80">
+      <c r="A80" s="14">
         <v>190497</v>
       </c>
       <c r="B80" s="3">
@@ -7468,7 +7465,7 @@
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A81">
+      <c r="A81" s="14">
         <v>191156</v>
       </c>
       <c r="B81" s="3">
@@ -7479,7 +7476,7 @@
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A82">
+      <c r="A82" s="14">
         <v>192696</v>
       </c>
       <c r="B82" s="3">
@@ -7490,7 +7487,7 @@
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A83">
+      <c r="A83" s="14">
         <v>193354</v>
       </c>
       <c r="B83" s="3">
@@ -7501,7 +7498,7 @@
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A84">
+      <c r="A84" s="14">
         <v>193684</v>
       </c>
       <c r="B84" s="3">
@@ -7515,7 +7512,7 @@
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A85">
+      <c r="A85" s="14">
         <v>193647</v>
       </c>
       <c r="B85" s="3">
@@ -7526,7 +7523,7 @@
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A86">
+      <c r="A86" s="14">
         <v>192067</v>
       </c>
       <c r="B86" s="3">
@@ -7537,7 +7534,7 @@
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A87">
+      <c r="A87" s="14">
         <v>193079</v>
       </c>
       <c r="B87" s="3">
@@ -7548,7 +7545,7 @@
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A88">
+      <c r="A88" s="14">
         <v>193672</v>
       </c>
       <c r="B88" s="3">
@@ -7559,7 +7556,7 @@
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A89">
+      <c r="A89" s="14">
         <v>193454</v>
       </c>
       <c r="B89" s="3">
@@ -7570,7 +7567,7 @@
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A90">
+      <c r="A90" s="14">
         <v>193536</v>
       </c>
       <c r="B90" s="3">
@@ -7584,7 +7581,7 @@
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A91">
+      <c r="A91" s="14">
         <v>193768</v>
       </c>
       <c r="B91" s="3">
@@ -7595,7 +7592,7 @@
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A92">
+      <c r="A92" s="14">
         <v>193236</v>
       </c>
       <c r="B92" s="3">
@@ -7606,7 +7603,7 @@
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A93">
+      <c r="A93" s="14">
         <v>193247</v>
       </c>
       <c r="B93" s="3">
@@ -7617,7 +7614,7 @@
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A94">
+      <c r="A94" s="14">
         <v>193278</v>
       </c>
       <c r="B94" s="3">
@@ -7628,7 +7625,7 @@
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A95">
+      <c r="A95" s="14">
         <v>193279</v>
       </c>
       <c r="B95" s="3">
@@ -7639,7 +7636,7 @@
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A96">
+      <c r="A96" s="14">
         <v>193280</v>
       </c>
       <c r="B96" s="3">
@@ -7650,7 +7647,7 @@
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A97">
+      <c r="A97" s="14">
         <v>193281</v>
       </c>
       <c r="B97" s="3">
@@ -7661,7 +7658,7 @@
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A98">
+      <c r="A98" s="14">
         <v>193645</v>
       </c>
       <c r="B98" s="3">
@@ -7672,7 +7669,7 @@
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A99">
+      <c r="A99" s="14">
         <v>191472</v>
       </c>
       <c r="B99" s="3">
@@ -7683,7 +7680,7 @@
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A100">
+      <c r="A100" s="14">
         <v>194379</v>
       </c>
       <c r="B100" s="3">
@@ -7694,7 +7691,7 @@
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A101">
+      <c r="A101" s="14">
         <v>193504</v>
       </c>
       <c r="B101" s="3">
@@ -7705,7 +7702,7 @@
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A102">
+      <c r="A102" s="14">
         <v>193731</v>
       </c>
       <c r="B102" s="3">
@@ -7716,7 +7713,7 @@
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A103">
+      <c r="A103" s="14">
         <v>193867</v>
       </c>
       <c r="B103" s="3">
@@ -7727,7 +7724,7 @@
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A104">
+      <c r="A104" s="14">
         <v>193922</v>
       </c>
       <c r="B104" s="3">
@@ -7738,7 +7735,7 @@
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A105">
+      <c r="A105" s="14">
         <v>193990</v>
       </c>
       <c r="B105" s="3">
@@ -7749,7 +7746,7 @@
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A106">
+      <c r="A106" s="14">
         <v>193753</v>
       </c>
       <c r="B106" s="3">
@@ -7760,7 +7757,7 @@
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A107">
+      <c r="A107" s="14">
         <v>193754</v>
       </c>
       <c r="B107" s="3">
@@ -7771,7 +7768,7 @@
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A108">
+      <c r="A108" s="14">
         <v>189445</v>
       </c>
       <c r="B108" s="3">
@@ -7782,7 +7779,7 @@
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A109">
+      <c r="A109" s="14">
         <v>191469</v>
       </c>
       <c r="B109" s="3">
@@ -7793,7 +7790,7 @@
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A110">
+      <c r="A110" s="14">
         <v>191470</v>
       </c>
       <c r="B110" s="3">
@@ -7807,7 +7804,7 @@
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A111">
+      <c r="A111" s="14">
         <v>191471</v>
       </c>
       <c r="B111" s="3">
@@ -7818,7 +7815,7 @@
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A112">
+      <c r="A112" s="14">
         <v>191473</v>
       </c>
       <c r="B112" s="3">
@@ -7829,7 +7826,7 @@
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A113">
+      <c r="A113" s="14">
         <v>191614</v>
       </c>
       <c r="B113" s="3">
@@ -7843,7 +7840,7 @@
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A114">
+      <c r="A114" s="14">
         <v>191766</v>
       </c>
       <c r="B114" s="3">
@@ -7854,7 +7851,7 @@
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A115">
+      <c r="A115" s="14">
         <v>191960</v>
       </c>
       <c r="B115" s="3">
@@ -7865,7 +7862,7 @@
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A116">
+      <c r="A116" s="14">
         <v>191961</v>
       </c>
       <c r="B116" s="3">
@@ -7876,7 +7873,7 @@
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A117">
+      <c r="A117" s="14">
         <v>191962</v>
       </c>
       <c r="B117" s="3">
@@ -7887,7 +7884,7 @@
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A118">
+      <c r="A118" s="14">
         <v>191993</v>
       </c>
       <c r="B118" s="3">
@@ -7898,7 +7895,7 @@
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A119">
+      <c r="A119" s="14">
         <v>192066</v>
       </c>
       <c r="B119" s="3">
@@ -7909,7 +7906,7 @@
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A120">
+      <c r="A120" s="14">
         <v>192286</v>
       </c>
       <c r="B120" s="3">
@@ -7920,7 +7917,7 @@
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A121">
+      <c r="A121" s="14">
         <v>193237</v>
       </c>
       <c r="B121" s="3">
@@ -7931,7 +7928,7 @@
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A122">
+      <c r="A122" s="14">
         <v>193305</v>
       </c>
       <c r="B122" s="3">
@@ -7942,7 +7939,7 @@
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A123">
+      <c r="A123" s="14">
         <v>193353</v>
       </c>
       <c r="B123" s="3">
@@ -7953,7 +7950,7 @@
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A124">
+      <c r="A124" s="14">
         <v>193697</v>
       </c>
       <c r="B124" s="3">
@@ -7964,7 +7961,7 @@
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A125">
+      <c r="A125" s="14">
         <v>193756</v>
       </c>
       <c r="B125" s="3">
@@ -7975,7 +7972,7 @@
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A126">
+      <c r="A126" s="14">
         <v>193984</v>
       </c>
       <c r="B126" s="3">
@@ -7986,7 +7983,7 @@
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A127">
+      <c r="A127" s="14">
         <v>193989</v>
       </c>
       <c r="B127" s="3">
@@ -7997,7 +7994,7 @@
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A128">
+      <c r="A128" s="14">
         <v>193994</v>
       </c>
       <c r="B128" s="3">
@@ -8008,7 +8005,7 @@
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A129">
+      <c r="A129" s="14">
         <v>194207</v>
       </c>
       <c r="B129" s="3">
@@ -8019,7 +8016,7 @@
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A130">
+      <c r="A130" s="14">
         <v>191958</v>
       </c>
       <c r="B130" s="3">
@@ -8030,7 +8027,7 @@
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A131">
+      <c r="A131" s="14">
         <v>193677</v>
       </c>
       <c r="B131" s="3">
@@ -8041,7 +8038,7 @@
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A132">
+      <c r="A132" s="14">
         <v>193884</v>
       </c>
       <c r="B132" s="3">
@@ -8052,7 +8049,7 @@
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A133">
+      <c r="A133" s="14">
         <v>193959</v>
       </c>
       <c r="B133" s="3">
@@ -8063,7 +8060,7 @@
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A134">
+      <c r="A134" s="14">
         <v>194108</v>
       </c>
       <c r="B134" s="3">
@@ -8074,7 +8071,7 @@
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A135">
+      <c r="A135" s="14">
         <v>194144</v>
       </c>
       <c r="B135" s="3">
@@ -8085,7 +8082,7 @@
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A136">
+      <c r="A136" s="14">
         <v>194145</v>
       </c>
       <c r="B136" s="3">
@@ -8096,7 +8093,7 @@
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A137">
+      <c r="A137" s="14">
         <v>194178</v>
       </c>
       <c r="B137" s="3">
@@ -8107,7 +8104,7 @@
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A138">
+      <c r="A138" s="14">
         <v>194284</v>
       </c>
       <c r="B138" s="3">
@@ -8118,7 +8115,7 @@
       </c>
     </row>
     <row r="139" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A139">
+      <c r="A139" s="14">
         <v>194289</v>
       </c>
       <c r="B139" s="3">
@@ -8129,7 +8126,7 @@
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A140">
+      <c r="A140" s="14">
         <v>191378</v>
       </c>
       <c r="B140" s="3">
@@ -8140,7 +8137,7 @@
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A141">
+      <c r="A141" s="14">
         <v>193885</v>
       </c>
       <c r="B141" s="3">
@@ -8151,7 +8148,7 @@
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A142">
+      <c r="A142" s="14">
         <v>193940</v>
       </c>
       <c r="B142" s="3">
@@ -8162,7 +8159,7 @@
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A143">
+      <c r="A143" s="14">
         <v>193374</v>
       </c>
       <c r="B143" s="3">
@@ -8173,7 +8170,7 @@
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A144">
+      <c r="A144" s="14">
         <v>194102</v>
       </c>
       <c r="B144" s="3">
@@ -8184,7 +8181,7 @@
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A145">
+      <c r="A145" s="14">
         <v>194323</v>
       </c>
       <c r="B145" s="3">
@@ -8195,7 +8192,7 @@
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A146">
+      <c r="A146" s="14">
         <v>194386</v>
       </c>
       <c r="B146" s="3">
@@ -8206,7 +8203,7 @@
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A147">
+      <c r="A147" s="14">
         <v>191996</v>
       </c>
       <c r="B147" s="3">
@@ -8217,7 +8214,7 @@
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A148">
+      <c r="A148" s="14">
         <v>194068</v>
       </c>
       <c r="B148" s="3">
@@ -8228,7 +8225,7 @@
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A149">
+      <c r="A149" s="14">
         <v>194333</v>
       </c>
       <c r="B149" s="3">
@@ -8239,7 +8236,7 @@
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A150">
+      <c r="A150" s="14">
         <v>193882</v>
       </c>
       <c r="B150" s="3">
@@ -8250,7 +8247,7 @@
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A151">
+      <c r="A151" s="14">
         <v>194336</v>
       </c>
       <c r="B151" s="3">
@@ -8261,7 +8258,7 @@
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A152">
+      <c r="A152" s="14">
         <v>194408</v>
       </c>
       <c r="B152" s="3">
@@ -8272,7 +8269,7 @@
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A153">
+      <c r="A153" s="14">
         <v>194468</v>
       </c>
       <c r="B153" s="3">
@@ -8283,7 +8280,7 @@
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A154">
+      <c r="A154" s="14">
         <v>194146</v>
       </c>
       <c r="B154" s="3">
@@ -8294,7 +8291,7 @@
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A155">
+      <c r="A155" s="14">
         <v>194272</v>
       </c>
       <c r="B155" s="3">
@@ -8308,7 +8305,7 @@
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A156">
+      <c r="A156" s="14">
         <v>194480</v>
       </c>
       <c r="B156" s="3">
@@ -8319,7 +8316,7 @@
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A157">
+      <c r="A157" s="14">
         <v>194492</v>
       </c>
       <c r="B157" s="3">
@@ -8330,7 +8327,7 @@
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A158">
+      <c r="A158" s="14">
         <v>191626</v>
       </c>
       <c r="B158" s="3">
@@ -8341,7 +8338,7 @@
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A159">
+      <c r="A159" s="14">
         <v>191826</v>
       </c>
       <c r="B159" s="3">
@@ -8352,7 +8349,7 @@
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A160">
+      <c r="A160" s="14">
         <v>192434</v>
       </c>
       <c r="B160" s="3">
@@ -8363,7 +8360,7 @@
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A161">
+      <c r="A161" s="14">
         <v>193288</v>
       </c>
       <c r="B161" s="3">
@@ -8374,7 +8371,7 @@
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A162">
+      <c r="A162" s="14">
         <v>193570</v>
       </c>
       <c r="B162" s="3">
@@ -8385,7 +8382,7 @@
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A163">
+      <c r="A163" s="14">
         <v>194083</v>
       </c>
       <c r="B163" s="3">
@@ -8396,7 +8393,7 @@
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A164">
+      <c r="A164" s="14">
         <v>194332</v>
       </c>
       <c r="B164" s="3">
@@ -8407,7 +8404,7 @@
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A165">
+      <c r="A165" s="14">
         <v>194387</v>
       </c>
       <c r="B165" s="3">
@@ -8418,7 +8415,7 @@
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A166">
+      <c r="A166" s="14">
         <v>194471</v>
       </c>
       <c r="B166" s="3">
@@ -8429,7 +8426,7 @@
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A167">
+      <c r="A167" s="14">
         <v>194481</v>
       </c>
       <c r="B167" s="3">
@@ -8440,7 +8437,7 @@
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A168">
+      <c r="A168" s="14">
         <v>194554</v>
       </c>
       <c r="B168" s="3">
@@ -8451,7 +8448,7 @@
       </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A169">
+      <c r="A169" s="14">
         <v>194555</v>
       </c>
       <c r="B169" s="3">
@@ -8462,7 +8459,7 @@
       </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A170">
+      <c r="A170" s="14">
         <v>194625</v>
       </c>
       <c r="B170" s="3">
@@ -8473,7 +8470,7 @@
       </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A171">
+      <c r="A171" s="14">
         <v>194388</v>
       </c>
       <c r="B171" s="3">
@@ -8484,7 +8481,7 @@
       </c>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A172">
+      <c r="A172" s="14">
         <v>194453</v>
       </c>
       <c r="B172" s="3">
@@ -8495,7 +8492,7 @@
       </c>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A173">
+      <c r="A173" s="14">
         <v>194513</v>
       </c>
       <c r="B173" s="3">
@@ -8506,7 +8503,7 @@
       </c>
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A174">
+      <c r="A174" s="14">
         <v>194762</v>
       </c>
       <c r="B174" s="3">
@@ -8517,7 +8514,7 @@
       </c>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A175">
+      <c r="A175" s="14">
         <v>194776</v>
       </c>
       <c r="B175" s="3">
@@ -8528,7 +8525,7 @@
       </c>
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A176">
+      <c r="A176" s="14">
         <v>194777</v>
       </c>
       <c r="B176" s="3">
@@ -8539,7 +8536,7 @@
       </c>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A177">
+      <c r="A177" s="14">
         <v>194214</v>
       </c>
       <c r="B177" s="3">
@@ -8550,7 +8547,7 @@
       </c>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A178">
+      <c r="A178" s="14">
         <v>194774</v>
       </c>
       <c r="B178" s="3">
@@ -8561,7 +8558,7 @@
       </c>
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A179">
+      <c r="A179" s="14">
         <v>195059</v>
       </c>
       <c r="B179" s="3">
@@ -8572,7 +8569,7 @@
       </c>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A180">
+      <c r="A180" s="14">
         <v>193621</v>
       </c>
       <c r="B180" s="3">
@@ -8583,7 +8580,7 @@
       </c>
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A181">
+      <c r="A181" s="14">
         <v>195135</v>
       </c>
       <c r="B181" s="3">
@@ -8594,7 +8591,7 @@
       </c>
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A182">
+      <c r="A182" s="14">
         <v>194099</v>
       </c>
       <c r="B182" s="3">
@@ -8605,7 +8602,7 @@
       </c>
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A183">
+      <c r="A183" s="14">
         <v>194563</v>
       </c>
       <c r="B183" s="3">
@@ -8616,7 +8613,7 @@
       </c>
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A184">
+      <c r="A184" s="14">
         <v>194741</v>
       </c>
       <c r="B184" s="3">
@@ -8627,7 +8624,7 @@
       </c>
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A185">
+      <c r="A185" s="14">
         <v>194778</v>
       </c>
       <c r="B185" s="3">
@@ -8638,7 +8635,7 @@
       </c>
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A186">
+      <c r="A186" s="14">
         <v>195252</v>
       </c>
       <c r="B186" s="3">
@@ -8649,7 +8646,7 @@
       </c>
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A187">
+      <c r="A187" s="14">
         <v>195248</v>
       </c>
       <c r="B187" s="3">
@@ -8660,7 +8657,7 @@
       </c>
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A188">
+      <c r="A188" s="14">
         <v>194114</v>
       </c>
       <c r="B188" s="3">
@@ -8671,7 +8668,7 @@
       </c>
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A189">
+      <c r="A189" s="14">
         <v>194297</v>
       </c>
       <c r="B189" s="3">
@@ -8682,7 +8679,7 @@
       </c>
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A190">
+      <c r="A190" s="14">
         <v>194298</v>
       </c>
       <c r="B190" s="3">
@@ -8693,7 +8690,7 @@
       </c>
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A191">
+      <c r="A191" s="14">
         <v>194538</v>
       </c>
       <c r="B191" s="3">
@@ -8704,7 +8701,7 @@
       </c>
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A192">
+      <c r="A192" s="14">
         <v>194773</v>
       </c>
       <c r="B192" s="3">
@@ -8715,7 +8712,7 @@
       </c>
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A193">
+      <c r="A193" s="14">
         <v>195344</v>
       </c>
       <c r="B193" s="3">
@@ -8726,7 +8723,7 @@
       </c>
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A194">
+      <c r="A194" s="14">
         <v>195407</v>
       </c>
       <c r="B194" s="3">
@@ -8737,7 +8734,7 @@
       </c>
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A195">
+      <c r="A195" s="14">
         <v>191535</v>
       </c>
       <c r="B195" s="3">
@@ -8748,7 +8745,7 @@
       </c>
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A196">
+      <c r="A196" s="14">
         <v>191785</v>
       </c>
       <c r="B196" s="3">
@@ -8762,7 +8759,7 @@
       </c>
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A197">
+      <c r="A197" s="14">
         <v>194758</v>
       </c>
       <c r="B197" s="3">
@@ -8773,7 +8770,7 @@
       </c>
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A198">
+      <c r="A198" s="14">
         <v>195487</v>
       </c>
       <c r="B198" s="3">
@@ -8784,7 +8781,7 @@
       </c>
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A199">
+      <c r="A199" s="14">
         <v>195366</v>
       </c>
       <c r="B199" s="3">
@@ -8795,7 +8792,7 @@
       </c>
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A200">
+      <c r="A200" s="14">
         <v>195377</v>
       </c>
       <c r="B200" s="3">
@@ -8806,7 +8803,7 @@
       </c>
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A201">
+      <c r="A201" s="14">
         <v>195390</v>
       </c>
       <c r="B201" s="3">
@@ -8817,7 +8814,7 @@
       </c>
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A202">
+      <c r="A202" s="14">
         <v>195549</v>
       </c>
       <c r="B202" s="3">
@@ -8828,7 +8825,7 @@
       </c>
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A203">
+      <c r="A203" s="14">
         <v>192172</v>
       </c>
       <c r="B203" s="3">
@@ -8839,7 +8836,7 @@
       </c>
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A204">
+      <c r="A204" s="14">
         <v>193437</v>
       </c>
       <c r="B204" s="3">
@@ -8850,7 +8847,7 @@
       </c>
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A205">
+      <c r="A205" s="14">
         <v>194084</v>
       </c>
       <c r="B205" s="3">
@@ -8861,7 +8858,7 @@
       </c>
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A206">
+      <c r="A206" s="14">
         <v>194391</v>
       </c>
       <c r="B206" s="3">
@@ -8872,7 +8869,7 @@
       </c>
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A207">
+      <c r="A207" s="14">
         <v>194612</v>
       </c>
       <c r="B207" s="3">
@@ -8883,7 +8880,7 @@
       </c>
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A208">
+      <c r="A208" s="14">
         <v>194751</v>
       </c>
       <c r="B208" s="3">
@@ -8894,7 +8891,7 @@
       </c>
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A209">
+      <c r="A209" s="14">
         <v>195058</v>
       </c>
       <c r="B209" s="3">
@@ -8905,7 +8902,7 @@
       </c>
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A210">
+      <c r="A210" s="14">
         <v>195230</v>
       </c>
       <c r="B210" s="3">
@@ -8916,7 +8913,7 @@
       </c>
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A211">
+      <c r="A211" s="14">
         <v>195264</v>
       </c>
       <c r="B211" s="3">
@@ -8927,7 +8924,7 @@
       </c>
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A212">
+      <c r="A212" s="14">
         <v>195271</v>
       </c>
       <c r="B212" s="3">
@@ -8938,7 +8935,7 @@
       </c>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A213">
+      <c r="A213" s="14">
         <v>195471</v>
       </c>
       <c r="B213" s="3">
@@ -8949,7 +8946,7 @@
       </c>
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A214">
+      <c r="A214" s="14">
         <v>195474</v>
       </c>
       <c r="B214" s="3">
@@ -8960,7 +8957,7 @@
       </c>
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A215">
+      <c r="A215" s="14">
         <v>195493</v>
       </c>
       <c r="B215" s="3">
@@ -8971,7 +8968,7 @@
       </c>
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A216">
+      <c r="A216" s="14">
         <v>195705</v>
       </c>
       <c r="B216" s="3">
@@ -8982,7 +8979,7 @@
       </c>
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A217">
+      <c r="A217" s="14">
         <v>195711</v>
       </c>
       <c r="B217" s="3">
@@ -8993,7 +8990,7 @@
       </c>
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A218">
+      <c r="A218" s="14">
         <v>195768</v>
       </c>
       <c r="B218" s="3">
@@ -9004,7 +9001,7 @@
       </c>
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A219">
+      <c r="A219" s="14">
         <v>194686</v>
       </c>
       <c r="B219" s="3">
@@ -9015,7 +9012,7 @@
       </c>
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A220">
+      <c r="A220" s="14">
         <v>194831</v>
       </c>
       <c r="B220" s="3">
@@ -9026,7 +9023,7 @@
       </c>
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A221">
+      <c r="A221" s="14">
         <v>195269</v>
       </c>
       <c r="B221" s="3">
@@ -9037,7 +9034,7 @@
       </c>
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A222">
+      <c r="A222" s="14">
         <v>195298</v>
       </c>
       <c r="B222" s="3">
@@ -9051,7 +9048,7 @@
       </c>
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A223">
+      <c r="A223" s="14">
         <v>194703</v>
       </c>
       <c r="B223" s="3">
@@ -9062,7 +9059,7 @@
       </c>
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A224">
+      <c r="A224" s="14">
         <v>195519</v>
       </c>
       <c r="B224" s="3">
@@ -9073,7 +9070,7 @@
       </c>
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A225">
+      <c r="A225" s="14">
         <v>195724</v>
       </c>
       <c r="B225" s="3">
@@ -9084,7 +9081,7 @@
       </c>
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A226">
+      <c r="A226" s="14">
         <v>195755</v>
       </c>
       <c r="B226" s="3">
@@ -9095,7 +9092,7 @@
       </c>
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A227">
+      <c r="A227" s="14">
         <v>195786</v>
       </c>
       <c r="B227" s="3">
@@ -9106,7 +9103,7 @@
       </c>
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A228">
+      <c r="A228" s="14">
         <v>195883</v>
       </c>
       <c r="B228" s="3">
@@ -9117,7 +9114,7 @@
       </c>
     </row>
     <row r="229" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A229">
+      <c r="A229" s="14">
         <v>195885</v>
       </c>
       <c r="B229" s="3">
@@ -9128,7 +9125,7 @@
       </c>
     </row>
     <row r="230" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A230">
+      <c r="A230" s="14">
         <v>195926</v>
       </c>
       <c r="B230" s="3">
@@ -9139,7 +9136,7 @@
       </c>
     </row>
     <row r="231" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A231">
+      <c r="A231" s="14">
         <v>195952</v>
       </c>
       <c r="B231" s="3">
@@ -9150,7 +9147,7 @@
       </c>
     </row>
     <row r="232" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A232">
+      <c r="A232" s="14">
         <v>195985</v>
       </c>
       <c r="B232" s="3">
@@ -9161,7 +9158,7 @@
       </c>
     </row>
     <row r="233" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A233">
+      <c r="A233" s="14">
         <v>195986</v>
       </c>
       <c r="B233" s="3">
@@ -9172,7 +9169,7 @@
       </c>
     </row>
     <row r="234" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A234">
+      <c r="A234" s="14">
         <v>195987</v>
       </c>
       <c r="B234" s="3">
@@ -9183,7 +9180,7 @@
       </c>
     </row>
     <row r="235" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A235">
+      <c r="A235" s="14">
         <v>195988</v>
       </c>
       <c r="B235" s="3">
@@ -9194,7 +9191,7 @@
       </c>
     </row>
     <row r="236" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A236">
+      <c r="A236" s="14">
         <v>195989</v>
       </c>
       <c r="B236" s="3">
@@ -9205,7 +9202,7 @@
       </c>
     </row>
     <row r="237" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A237">
+      <c r="A237" s="14">
         <v>195998</v>
       </c>
       <c r="B237" s="3">
@@ -9219,7 +9216,7 @@
       </c>
     </row>
     <row r="238" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A238">
+      <c r="A238" s="14">
         <v>194809</v>
       </c>
       <c r="B238" s="3">
@@ -9230,7 +9227,7 @@
       </c>
     </row>
     <row r="239" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A239">
+      <c r="A239" s="14">
         <v>195902</v>
       </c>
       <c r="B239" s="3">
@@ -9241,7 +9238,7 @@
       </c>
     </row>
     <row r="240" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A240">
+      <c r="A240" s="14">
         <v>192992</v>
       </c>
       <c r="B240" s="3">
@@ -9255,7 +9252,7 @@
       </c>
     </row>
     <row r="241" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A241">
+      <c r="A241" s="14">
         <v>193713</v>
       </c>
       <c r="B241" s="3">
@@ -9266,7 +9263,7 @@
       </c>
     </row>
     <row r="242" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A242">
+      <c r="A242" s="14">
         <v>194321</v>
       </c>
       <c r="B242" s="3">
@@ -9280,7 +9277,7 @@
       </c>
     </row>
     <row r="243" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A243">
+      <c r="A243" s="14">
         <v>195454</v>
       </c>
       <c r="B243" s="3">
@@ -9291,7 +9288,7 @@
       </c>
     </row>
     <row r="244" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A244">
+      <c r="A244" s="14">
         <v>195709</v>
       </c>
       <c r="B244" s="3">
@@ -9302,7 +9299,7 @@
       </c>
     </row>
     <row r="245" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A245">
+      <c r="A245" s="14">
         <v>195799</v>
       </c>
       <c r="B245" s="3">
@@ -9313,7 +9310,7 @@
       </c>
     </row>
     <row r="246" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A246">
+      <c r="A246" s="14">
         <v>195919</v>
       </c>
       <c r="B246" s="3">
@@ -9324,7 +9321,7 @@
       </c>
     </row>
     <row r="247" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A247">
+      <c r="A247" s="14">
         <v>195935</v>
       </c>
       <c r="B247" s="3">
@@ -9335,7 +9332,7 @@
       </c>
     </row>
     <row r="248" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A248">
+      <c r="A248" s="14">
         <v>196084</v>
       </c>
       <c r="B248" s="3">
@@ -9346,7 +9343,7 @@
       </c>
     </row>
     <row r="249" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A249">
+      <c r="A249" s="14">
         <v>196201</v>
       </c>
       <c r="B249" s="3">
@@ -9357,7 +9354,7 @@
       </c>
     </row>
     <row r="250" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A250">
+      <c r="A250" s="14">
         <v>195788</v>
       </c>
       <c r="B250" s="3">
@@ -9368,7 +9365,7 @@
       </c>
     </row>
     <row r="251" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A251">
+      <c r="A251" s="14">
         <v>195903</v>
       </c>
       <c r="B251" s="3">
@@ -9379,7 +9376,7 @@
       </c>
     </row>
     <row r="252" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A252">
+      <c r="A252" s="14">
         <v>196329</v>
       </c>
       <c r="B252" s="3">
@@ -9390,7 +9387,7 @@
       </c>
     </row>
     <row r="253" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A253">
+      <c r="A253" s="14">
         <v>196379</v>
       </c>
       <c r="B253" s="3">
@@ -9401,7 +9398,7 @@
       </c>
     </row>
     <row r="254" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A254">
+      <c r="A254" s="14">
         <v>196514</v>
       </c>
       <c r="B254" s="3">
@@ -9412,7 +9409,7 @@
       </c>
     </row>
     <row r="255" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A255">
+      <c r="A255" s="14">
         <v>196601</v>
       </c>
       <c r="B255" s="3">
@@ -9426,7 +9423,7 @@
       </c>
     </row>
     <row r="256" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A256">
+      <c r="A256" s="14">
         <v>195370</v>
       </c>
       <c r="B256" s="3">
@@ -9437,7 +9434,7 @@
       </c>
     </row>
     <row r="257" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A257">
+      <c r="A257" s="14">
         <v>195444</v>
       </c>
       <c r="B257" s="3">
@@ -9448,7 +9445,7 @@
       </c>
     </row>
     <row r="258" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A258">
+      <c r="A258" s="14">
         <v>195844</v>
       </c>
       <c r="B258" s="3">
@@ -9459,7 +9456,7 @@
       </c>
     </row>
     <row r="259" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A259">
+      <c r="A259" s="14">
         <v>195951</v>
       </c>
       <c r="B259" s="3">
@@ -9470,7 +9467,7 @@
       </c>
     </row>
     <row r="260" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A260">
+      <c r="A260" s="14">
         <v>196031</v>
       </c>
       <c r="B260" s="3">
@@ -9481,7 +9478,7 @@
       </c>
     </row>
     <row r="261" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A261">
+      <c r="A261" s="14">
         <v>196336</v>
       </c>
       <c r="B261" s="3">
@@ -9492,7 +9489,7 @@
       </c>
     </row>
     <row r="262" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A262">
+      <c r="A262" s="14">
         <v>196117</v>
       </c>
       <c r="B262" s="3">
@@ -9503,7 +9500,7 @@
       </c>
     </row>
     <row r="263" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A263">
+      <c r="A263" s="14">
         <v>196540</v>
       </c>
       <c r="B263" s="3">
@@ -9514,7 +9511,7 @@
       </c>
     </row>
     <row r="264" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A264">
+      <c r="A264" s="14">
         <v>196653</v>
       </c>
       <c r="B264" s="3">
@@ -9525,7 +9522,7 @@
       </c>
     </row>
     <row r="265" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A265">
+      <c r="A265" s="14">
         <v>196655</v>
       </c>
       <c r="B265" s="3">
@@ -9536,7 +9533,7 @@
       </c>
     </row>
     <row r="266" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A266">
+      <c r="A266" s="14">
         <v>196683</v>
       </c>
       <c r="B266" s="3">
@@ -9547,7 +9544,7 @@
       </c>
     </row>
     <row r="267" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A267">
+      <c r="A267" s="14">
         <v>196687</v>
       </c>
       <c r="B267" s="3">
@@ -9558,7 +9555,7 @@
       </c>
     </row>
     <row r="268" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A268">
+      <c r="A268" s="14">
         <v>196771</v>
       </c>
       <c r="B268" s="3">
@@ -9569,7 +9566,7 @@
       </c>
     </row>
     <row r="269" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A269">
+      <c r="A269" s="14">
         <v>196774</v>
       </c>
       <c r="B269" s="3">
@@ -9580,7 +9577,7 @@
       </c>
     </row>
     <row r="270" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A270">
+      <c r="A270" s="14">
         <v>196797</v>
       </c>
       <c r="B270" s="3">
@@ -9591,7 +9588,7 @@
       </c>
     </row>
     <row r="271" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A271">
+      <c r="A271" s="14">
         <v>196890</v>
       </c>
       <c r="B271" s="3">
@@ -9602,7 +9599,7 @@
       </c>
     </row>
     <row r="272" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A272">
+      <c r="A272" s="14">
         <v>194321</v>
       </c>
       <c r="B272" s="3">
@@ -9613,7 +9610,7 @@
       </c>
     </row>
     <row r="273" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A273">
+      <c r="A273" s="14">
         <v>195389</v>
       </c>
       <c r="B273" s="3">
@@ -9624,7 +9621,7 @@
       </c>
     </row>
     <row r="274" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A274">
+      <c r="A274" s="14">
         <v>196560</v>
       </c>
       <c r="B274" s="3">
@@ -9635,7 +9632,7 @@
       </c>
     </row>
     <row r="275" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A275">
+      <c r="A275" s="14">
         <v>196741</v>
       </c>
       <c r="B275" s="3">
@@ -9646,7 +9643,7 @@
       </c>
     </row>
     <row r="276" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A276">
+      <c r="A276" s="14">
         <v>195994</v>
       </c>
       <c r="B276" s="3">
@@ -9657,7 +9654,7 @@
       </c>
     </row>
     <row r="277" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A277">
+      <c r="A277" s="14">
         <v>196341</v>
       </c>
       <c r="B277" s="3">
@@ -9668,7 +9665,7 @@
       </c>
     </row>
     <row r="278" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A278">
+      <c r="A278" s="14">
         <v>196528</v>
       </c>
       <c r="B278" s="3">
@@ -9679,7 +9676,7 @@
       </c>
     </row>
     <row r="279" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A279">
+      <c r="A279" s="14">
         <v>196744</v>
       </c>
       <c r="B279" s="3">
@@ -9690,7 +9687,7 @@
       </c>
     </row>
     <row r="280" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A280">
+      <c r="A280" s="14">
         <v>196875</v>
       </c>
       <c r="B280" s="3">
@@ -9701,7 +9698,7 @@
       </c>
     </row>
     <row r="281" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A281">
+      <c r="A281" s="14">
         <v>196916</v>
       </c>
       <c r="B281" s="3">
@@ -9712,7 +9709,7 @@
       </c>
     </row>
     <row r="282" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A282">
+      <c r="A282" s="14">
         <v>196933</v>
       </c>
       <c r="B282" s="3">
@@ -9723,7 +9720,7 @@
       </c>
     </row>
     <row r="283" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A283">
+      <c r="A283" s="14">
         <v>196937</v>
       </c>
       <c r="B283" s="3">
@@ -9734,7 +9731,7 @@
       </c>
     </row>
     <row r="284" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A284">
+      <c r="A284" s="14">
         <v>196977</v>
       </c>
       <c r="B284" s="3">
@@ -9745,7 +9742,7 @@
       </c>
     </row>
     <row r="285" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A285">
+      <c r="A285" s="14">
         <v>197074</v>
       </c>
       <c r="B285" s="3">
@@ -9756,7 +9753,7 @@
       </c>
     </row>
     <row r="286" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A286">
+      <c r="A286" s="14">
         <v>194721</v>
       </c>
       <c r="B286" s="3">
@@ -9767,7 +9764,7 @@
       </c>
     </row>
     <row r="287" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A287">
+      <c r="A287" s="14">
         <v>195934</v>
       </c>
       <c r="B287" s="3">
@@ -9778,7 +9775,7 @@
       </c>
     </row>
     <row r="288" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A288">
+      <c r="A288" s="14">
         <v>196235</v>
       </c>
       <c r="B288" s="3">
@@ -9789,7 +9786,7 @@
       </c>
     </row>
     <row r="289" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A289">
+      <c r="A289" s="14">
         <v>196408</v>
       </c>
       <c r="B289" s="3">
@@ -9800,7 +9797,7 @@
       </c>
     </row>
     <row r="290" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A290">
+      <c r="A290" s="14">
         <v>196709</v>
       </c>
       <c r="B290" s="3">
@@ -9811,7 +9808,7 @@
       </c>
     </row>
     <row r="291" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A291">
+      <c r="A291" s="14">
         <v>196737</v>
       </c>
       <c r="B291" s="3">
@@ -9822,7 +9819,7 @@
       </c>
     </row>
     <row r="292" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A292">
+      <c r="A292" s="14">
         <v>196769</v>
       </c>
       <c r="B292" s="3">
@@ -9833,7 +9830,7 @@
       </c>
     </row>
     <row r="293" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A293">
+      <c r="A293" s="14">
         <v>196908</v>
       </c>
       <c r="B293" s="3">
@@ -9844,7 +9841,7 @@
       </c>
     </row>
     <row r="294" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A294">
+      <c r="A294" s="14">
         <v>197059</v>
       </c>
       <c r="B294" s="3">
@@ -9855,7 +9852,7 @@
       </c>
     </row>
     <row r="295" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A295">
+      <c r="A295" s="14">
         <v>197065</v>
       </c>
       <c r="B295" s="3">
@@ -9866,7 +9863,7 @@
       </c>
     </row>
     <row r="296" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A296">
+      <c r="A296" s="14">
         <v>197077</v>
       </c>
       <c r="B296" s="3">
@@ -9877,7 +9874,7 @@
       </c>
     </row>
     <row r="297" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A297">
+      <c r="A297" s="14">
         <v>196768</v>
       </c>
       <c r="B297" s="3">
@@ -9888,7 +9885,7 @@
       </c>
     </row>
     <row r="298" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A298">
+      <c r="A298" s="14">
         <v>197239</v>
       </c>
       <c r="B298" s="3">
@@ -9899,7 +9896,7 @@
       </c>
     </row>
     <row r="299" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A299">
+      <c r="A299" s="14">
         <v>197256</v>
       </c>
       <c r="B299" s="3">
@@ -9910,7 +9907,7 @@
       </c>
     </row>
     <row r="300" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A300">
+      <c r="A300" s="14">
         <v>197295</v>
       </c>
       <c r="B300" s="3">
@@ -9921,7 +9918,7 @@
       </c>
     </row>
     <row r="301" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A301">
+      <c r="A301" s="14">
         <v>195292</v>
       </c>
       <c r="B301" s="3">
@@ -9935,7 +9932,7 @@
       </c>
     </row>
     <row r="302" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A302">
+      <c r="A302" s="14">
         <v>195299</v>
       </c>
       <c r="B302" s="3">
@@ -9949,7 +9946,7 @@
       </c>
     </row>
     <row r="303" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A303">
+      <c r="A303" s="14">
         <v>195694</v>
       </c>
       <c r="B303" s="3">
@@ -9963,7 +9960,7 @@
       </c>
     </row>
     <row r="304" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A304">
+      <c r="A304" s="14">
         <v>195706</v>
       </c>
       <c r="B304" s="3">
@@ -9977,7 +9974,7 @@
       </c>
     </row>
     <row r="305" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A305">
+      <c r="A305" s="14">
         <v>196190</v>
       </c>
       <c r="B305" s="3">
@@ -9988,7 +9985,7 @@
       </c>
     </row>
     <row r="306" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A306">
+      <c r="A306" s="14">
         <v>196419</v>
       </c>
       <c r="B306" s="3">
@@ -10002,7 +9999,7 @@
       </c>
     </row>
     <row r="307" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A307">
+      <c r="A307" s="14">
         <v>196672</v>
       </c>
       <c r="B307" s="3">
@@ -10013,7 +10010,7 @@
       </c>
     </row>
     <row r="308" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A308">
+      <c r="A308" s="14">
         <v>196852</v>
       </c>
       <c r="B308" s="3">
@@ -10024,7 +10021,7 @@
       </c>
     </row>
     <row r="309" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A309">
+      <c r="A309" s="14">
         <v>197303</v>
       </c>
       <c r="B309" s="3">
@@ -10038,7 +10035,7 @@
       </c>
     </row>
     <row r="310" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A310">
+      <c r="A310" s="14">
         <v>197601</v>
       </c>
       <c r="B310" s="3">
@@ -10049,7 +10046,7 @@
       </c>
     </row>
     <row r="311" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A311">
+      <c r="A311" s="14">
         <v>197628</v>
       </c>
       <c r="B311" s="3">
@@ -10060,7 +10057,7 @@
       </c>
     </row>
     <row r="312" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A312">
+      <c r="A312" s="14">
         <v>195541</v>
       </c>
       <c r="B312" s="3">
@@ -10071,7 +10068,7 @@
       </c>
     </row>
     <row r="313" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A313">
+      <c r="A313" s="14">
         <v>195589</v>
       </c>
       <c r="B313" s="3">
@@ -10082,7 +10079,7 @@
       </c>
     </row>
     <row r="314" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A314">
+      <c r="A314" s="14">
         <v>196376</v>
       </c>
       <c r="B314" s="3">
@@ -10093,7 +10090,7 @@
       </c>
     </row>
     <row r="315" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A315">
+      <c r="A315" s="14">
         <v>196824</v>
       </c>
       <c r="B315" s="3">
@@ -10104,7 +10101,7 @@
       </c>
     </row>
     <row r="316" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A316">
+      <c r="A316" s="14">
         <v>197558</v>
       </c>
       <c r="B316" s="3">
@@ -10115,7 +10112,7 @@
       </c>
     </row>
     <row r="317" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A317">
+      <c r="A317" s="14">
         <v>195265</v>
       </c>
       <c r="B317" s="3">
@@ -10126,7 +10123,7 @@
       </c>
     </row>
     <row r="318" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A318">
+      <c r="A318" s="14">
         <v>195266</v>
       </c>
       <c r="B318" s="3">
@@ -10137,7 +10134,7 @@
       </c>
     </row>
     <row r="319" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A319">
+      <c r="A319" s="14">
         <v>195360</v>
       </c>
       <c r="B319" s="3">
@@ -10148,7 +10145,7 @@
       </c>
     </row>
     <row r="320" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A320">
+      <c r="A320" s="14">
         <v>196287</v>
       </c>
       <c r="B320" s="3">
@@ -10159,7 +10156,7 @@
       </c>
     </row>
     <row r="321" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A321">
+      <c r="A321" s="14">
         <v>197721</v>
       </c>
       <c r="B321" s="3">
@@ -10170,7 +10167,7 @@
       </c>
     </row>
     <row r="322" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A322">
+      <c r="A322" s="14">
         <v>197888</v>
       </c>
       <c r="B322" s="3">
@@ -10181,7 +10178,7 @@
       </c>
     </row>
     <row r="323" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A323">
+      <c r="A323" s="14">
         <v>194317</v>
       </c>
       <c r="B323" s="3">
@@ -10192,7 +10189,7 @@
       </c>
     </row>
     <row r="324" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A324">
+      <c r="A324" s="14">
         <v>195864</v>
       </c>
       <c r="B324" s="3">
@@ -10203,7 +10200,7 @@
       </c>
     </row>
     <row r="325" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A325">
+      <c r="A325" s="14">
         <v>198004</v>
       </c>
       <c r="B325" s="3">
@@ -10214,7 +10211,7 @@
       </c>
     </row>
     <row r="326" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A326">
+      <c r="A326" s="14">
         <v>197707</v>
       </c>
       <c r="B326" s="3">
@@ -10225,7 +10222,7 @@
       </c>
     </row>
     <row r="327" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A327">
+      <c r="A327" s="14">
         <v>196650</v>
       </c>
       <c r="B327" s="3">
@@ -10239,7 +10236,7 @@
       </c>
     </row>
     <row r="328" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A328">
+      <c r="A328" s="14">
         <v>197985</v>
       </c>
       <c r="B328" s="3">
@@ -10250,7 +10247,7 @@
       </c>
     </row>
     <row r="329" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A329">
+      <c r="A329" s="14">
         <v>198148</v>
       </c>
       <c r="B329" s="3">
@@ -10269,7 +10266,7 @@
   </sortState>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="landscape" verticalDpi="0" copies="2" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="landscape" verticalDpi="200" copies="2" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -10278,18 +10275,19 @@
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
+    <col min="1" max="1" width="9" style="14"/>
     <col min="2" max="2" width="13.25" customWidth="1"/>
     <col min="3" max="3" width="10.5" style="3" customWidth="1"/>
     <col min="4" max="4" width="19.875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="13" t="s">
         <v>19</v>
       </c>
       <c r="B1" s="2" t="s">
@@ -10306,7 +10304,7 @@
       <c r="H1" s="5"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A2">
+      <c r="A2" s="14">
         <v>197066</v>
       </c>
       <c r="B2" s="3">
@@ -10314,7 +10312,7 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A3">
+      <c r="A3" s="14">
         <v>197132</v>
       </c>
       <c r="B3" s="3">
@@ -10322,7 +10320,7 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A4">
+      <c r="A4" s="14">
         <v>197157</v>
       </c>
       <c r="B4" s="3">
@@ -10330,7 +10328,7 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A5">
+      <c r="A5" s="14">
         <v>197297</v>
       </c>
       <c r="B5" s="3">
@@ -10338,7 +10336,7 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A6">
+      <c r="A6" s="14">
         <v>197683</v>
       </c>
       <c r="B6" s="3">
@@ -10346,7 +10344,7 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A7">
+      <c r="A7" s="14">
         <v>197837</v>
       </c>
       <c r="B7" s="3">
@@ -10354,7 +10352,7 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A8">
+      <c r="A8" s="14">
         <v>198058</v>
       </c>
       <c r="B8" s="3">
@@ -10362,7 +10360,7 @@
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A9">
+      <c r="A9" s="14">
         <v>198223</v>
       </c>
       <c r="B9" s="3">
@@ -10370,7 +10368,7 @@
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A10">
+      <c r="A10" s="14">
         <v>198224</v>
       </c>
       <c r="B10" s="3">
@@ -10378,7 +10376,7 @@
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A11">
+      <c r="A11" s="14">
         <v>198254</v>
       </c>
       <c r="B11" s="3">
@@ -10386,7 +10384,7 @@
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A12">
+      <c r="A12" s="14">
         <v>198259</v>
       </c>
       <c r="B12" s="3">
@@ -10408,17 +10406,18 @@
   <dimension ref="A1:D99"/>
   <sheetViews>
     <sheetView topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="A99" sqref="A99:XFD99"/>
+      <selection activeCell="A85" sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
+    <col min="1" max="1" width="9" style="14"/>
     <col min="2" max="2" width="11.625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.625" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="13" t="s">
         <v>19</v>
       </c>
       <c r="B1" s="2" t="s">
@@ -10429,7 +10428,7 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A2">
+      <c r="A2" s="14">
         <v>183311</v>
       </c>
       <c r="B2" s="3">
@@ -10440,7 +10439,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A3">
+      <c r="A3" s="14">
         <v>191292</v>
       </c>
       <c r="B3" s="3">
@@ -10451,7 +10450,7 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A4">
+      <c r="A4" s="14">
         <v>191375</v>
       </c>
       <c r="B4" s="3">
@@ -10462,7 +10461,7 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A5">
+      <c r="A5" s="14">
         <v>189981</v>
       </c>
       <c r="B5" s="3">
@@ -10473,7 +10472,7 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A6">
+      <c r="A6" s="14">
         <v>192739</v>
       </c>
       <c r="B6" s="3">
@@ -10484,7 +10483,7 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A7">
+      <c r="A7" s="14">
         <v>192789</v>
       </c>
       <c r="B7" s="3">
@@ -10495,7 +10494,7 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A8">
+      <c r="A8" s="14">
         <v>191407</v>
       </c>
       <c r="B8" s="3">
@@ -10509,7 +10508,7 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A9">
+      <c r="A9" s="14">
         <v>193060</v>
       </c>
       <c r="B9" s="3">
@@ -10520,7 +10519,7 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A10">
+      <c r="A10" s="14">
         <v>192996</v>
       </c>
       <c r="B10" s="3">
@@ -10531,7 +10530,7 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A11">
+      <c r="A11" s="14">
         <v>193174</v>
       </c>
       <c r="B11" s="3">
@@ -10542,7 +10541,7 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A12">
+      <c r="A12" s="14">
         <v>191626</v>
       </c>
       <c r="B12" s="3">
@@ -10556,7 +10555,7 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A13">
+      <c r="A13" s="14">
         <v>192066</v>
       </c>
       <c r="B13" s="3">
@@ -10570,7 +10569,7 @@
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A14">
+      <c r="A14" s="14">
         <v>192067</v>
       </c>
       <c r="B14" s="3">
@@ -10584,7 +10583,7 @@
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A15">
+      <c r="A15" s="14">
         <v>193370</v>
       </c>
       <c r="B15" s="3">
@@ -10595,7 +10594,7 @@
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A16">
+      <c r="A16" s="14">
         <v>193392</v>
       </c>
       <c r="B16" s="3">
@@ -10606,7 +10605,7 @@
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A17">
+      <c r="A17" s="14">
         <v>193368</v>
       </c>
       <c r="B17" s="3">
@@ -10617,7 +10616,7 @@
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A18">
+      <c r="A18" s="14">
         <v>193439</v>
       </c>
       <c r="B18" s="3">
@@ -10628,7 +10627,7 @@
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A19">
+      <c r="A19" s="14">
         <v>193438</v>
       </c>
       <c r="B19" s="3">
@@ -10639,7 +10638,7 @@
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A20">
+      <c r="A20" s="14">
         <v>193456</v>
       </c>
       <c r="B20" s="3">
@@ -10650,7 +10649,7 @@
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A21">
+      <c r="A21" s="14">
         <v>193455</v>
       </c>
       <c r="B21" s="3">
@@ -10661,7 +10660,7 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A22">
+      <c r="A22" s="14">
         <v>193504</v>
       </c>
       <c r="B22" s="3">
@@ -10675,7 +10674,7 @@
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A23">
+      <c r="A23" s="14">
         <v>193556</v>
       </c>
       <c r="B23" s="3">
@@ -10686,7 +10685,7 @@
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A24">
+      <c r="A24" s="14">
         <v>193453</v>
       </c>
       <c r="B24" s="3">
@@ -10697,7 +10696,7 @@
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A25">
+      <c r="A25" s="14">
         <v>193514</v>
       </c>
       <c r="B25" s="3">
@@ -10708,7 +10707,7 @@
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A26">
+      <c r="A26" s="14">
         <v>193515</v>
       </c>
       <c r="B26" s="3">
@@ -10719,7 +10718,7 @@
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A27">
+      <c r="A27" s="14">
         <v>193516</v>
       </c>
       <c r="B27" s="3">
@@ -10730,7 +10729,7 @@
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A28">
+      <c r="A28" s="14">
         <v>193535</v>
       </c>
       <c r="B28" s="3">
@@ -10741,7 +10740,7 @@
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A29">
+      <c r="A29" s="14">
         <v>193684</v>
       </c>
       <c r="B29" s="3">
@@ -10752,7 +10751,7 @@
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A30">
+      <c r="A30" s="14">
         <v>193786</v>
       </c>
       <c r="B30" s="3">
@@ -10763,7 +10762,7 @@
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A31">
+      <c r="A31" s="14">
         <v>193959</v>
       </c>
       <c r="B31" s="3">
@@ -10777,7 +10776,7 @@
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A32">
+      <c r="A32" s="14">
         <v>181638</v>
       </c>
       <c r="B32" s="3">
@@ -10788,7 +10787,7 @@
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A33">
+      <c r="A33" s="14">
         <v>193536</v>
       </c>
       <c r="B33" s="3">
@@ -10802,7 +10801,7 @@
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A34">
+      <c r="A34" s="14">
         <v>193518</v>
       </c>
       <c r="B34" s="3">
@@ -10813,7 +10812,7 @@
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A35">
+      <c r="A35" s="14">
         <v>193620</v>
       </c>
       <c r="B35" s="3">
@@ -10824,7 +10823,7 @@
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A36">
+      <c r="A36" s="14">
         <v>193728</v>
       </c>
       <c r="B36" s="3">
@@ -10835,7 +10834,7 @@
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A37">
+      <c r="A37" s="14">
         <v>194142</v>
       </c>
       <c r="B37" s="3">
@@ -10846,7 +10845,7 @@
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A38">
+      <c r="A38" s="14">
         <v>193926</v>
       </c>
       <c r="B38" s="3">
@@ -10857,7 +10856,7 @@
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A39">
+      <c r="A39" s="14">
         <v>194240</v>
       </c>
       <c r="B39" s="3">
@@ -10868,7 +10867,7 @@
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A40">
+      <c r="A40" s="14">
         <v>194267</v>
       </c>
       <c r="B40" s="3">
@@ -10879,7 +10878,7 @@
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A41">
+      <c r="A41" s="14">
         <v>194269</v>
       </c>
       <c r="B41" s="3">
@@ -10890,7 +10889,7 @@
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A42">
+      <c r="A42" s="14">
         <v>194270</v>
       </c>
       <c r="B42" s="3">
@@ -10901,7 +10900,7 @@
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A43">
+      <c r="A43" s="14">
         <v>194195</v>
       </c>
       <c r="B43" s="3">
@@ -10912,7 +10911,7 @@
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A44">
+      <c r="A44" s="14">
         <v>194383</v>
       </c>
       <c r="B44" s="3">
@@ -10923,7 +10922,7 @@
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A45">
+      <c r="A45" s="14">
         <v>194384</v>
       </c>
       <c r="B45" s="3">
@@ -10934,7 +10933,7 @@
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A46">
+      <c r="A46" s="14">
         <v>194513</v>
       </c>
       <c r="B46" s="3">
@@ -10948,7 +10947,7 @@
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A47">
+      <c r="A47" s="14">
         <v>194545</v>
       </c>
       <c r="B47" s="3">
@@ -10959,7 +10958,7 @@
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A48">
+      <c r="A48" s="14">
         <v>194546</v>
       </c>
       <c r="B48" s="3">
@@ -10970,7 +10969,7 @@
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A49">
+      <c r="A49" s="14">
         <v>194235</v>
       </c>
       <c r="B49" s="3">
@@ -10981,7 +10980,7 @@
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A50">
+      <c r="A50" s="14">
         <v>194351</v>
       </c>
       <c r="B50" s="3">
@@ -10992,7 +10991,7 @@
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A51">
+      <c r="A51" s="14">
         <v>194581</v>
       </c>
       <c r="B51" s="3">
@@ -11003,7 +11002,7 @@
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A52">
+      <c r="A52" s="14">
         <v>193762</v>
       </c>
       <c r="B52" s="3">
@@ -11014,7 +11013,7 @@
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A53">
+      <c r="A53" s="14">
         <v>191470</v>
       </c>
       <c r="B53" s="3">
@@ -11025,7 +11024,7 @@
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A54">
+      <c r="A54" s="14">
         <v>194714</v>
       </c>
       <c r="B54" s="3">
@@ -11036,7 +11035,7 @@
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A55">
+      <c r="A55" s="14">
         <v>194835</v>
       </c>
       <c r="B55" s="3">
@@ -11047,7 +11046,7 @@
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A56">
+      <c r="A56" s="14">
         <v>194862</v>
       </c>
       <c r="B56" s="3">
@@ -11058,7 +11057,7 @@
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A57">
+      <c r="A57" s="14">
         <v>194455</v>
       </c>
       <c r="B57" s="3">
@@ -11069,7 +11068,7 @@
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A58">
+      <c r="A58" s="14">
         <v>194456</v>
       </c>
       <c r="B58" s="3">
@@ -11080,7 +11079,7 @@
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A59">
+      <c r="A59" s="14">
         <v>194457</v>
       </c>
       <c r="B59" s="3">
@@ -11091,7 +11090,7 @@
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A60">
+      <c r="A60" s="14">
         <v>194458</v>
       </c>
       <c r="B60" s="3">
@@ -11102,7 +11101,7 @@
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A61">
+      <c r="A61" s="14">
         <v>194712</v>
       </c>
       <c r="B61" s="3">
@@ -11113,7 +11112,7 @@
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A62">
+      <c r="A62" s="14">
         <v>194713</v>
       </c>
       <c r="B62" s="3">
@@ -11124,7 +11123,7 @@
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A63">
+      <c r="A63" s="14">
         <v>194728</v>
       </c>
       <c r="B63" s="3">
@@ -11135,7 +11134,7 @@
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A64">
+      <c r="A64" s="14">
         <v>195431</v>
       </c>
       <c r="B64" s="3">
@@ -11146,7 +11145,7 @@
       </c>
     </row>
     <row r="65" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A65">
+      <c r="A65" s="14">
         <v>194272</v>
       </c>
       <c r="B65" s="3">
@@ -11160,7 +11159,7 @@
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A66">
+      <c r="A66" s="14">
         <v>194931</v>
       </c>
       <c r="B66" s="3">
@@ -11171,7 +11170,7 @@
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A67">
+      <c r="A67" s="14">
         <v>194659</v>
       </c>
       <c r="B67" s="3">
@@ -11182,7 +11181,7 @@
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A68">
+      <c r="A68" s="14">
         <v>195579</v>
       </c>
       <c r="B68" s="3">
@@ -11193,7 +11192,7 @@
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A69">
+      <c r="A69" s="14">
         <v>195582</v>
       </c>
       <c r="B69" s="3">
@@ -11204,7 +11203,7 @@
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A70">
+      <c r="A70" s="14">
         <v>193517</v>
       </c>
       <c r="B70" s="3">
@@ -11215,7 +11214,7 @@
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A71">
+      <c r="A71" s="14">
         <v>195359</v>
       </c>
       <c r="B71" s="3">
@@ -11226,7 +11225,7 @@
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A72">
+      <c r="A72" s="14">
         <v>195397</v>
       </c>
       <c r="B72" s="3">
@@ -11237,7 +11236,7 @@
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A73">
+      <c r="A73" s="14">
         <v>195726</v>
       </c>
       <c r="B73" s="3">
@@ -11248,7 +11247,7 @@
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A74">
+      <c r="A74" s="14">
         <v>195839</v>
       </c>
       <c r="B74" s="3">
@@ -11259,7 +11258,7 @@
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A75">
+      <c r="A75" s="14">
         <v>196239</v>
       </c>
       <c r="B75" s="3">
@@ -11270,7 +11269,7 @@
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A76">
+      <c r="A76" s="14">
         <v>194711</v>
       </c>
       <c r="B76" s="3">
@@ -11281,7 +11280,7 @@
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A77">
+      <c r="A77" s="14">
         <v>196061</v>
       </c>
       <c r="B77" s="3">
@@ -11292,7 +11291,7 @@
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A78">
+      <c r="A78" s="14">
         <v>196361</v>
       </c>
       <c r="B78" s="3">
@@ -11303,7 +11302,7 @@
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A79">
+      <c r="A79" s="14">
         <v>196663</v>
       </c>
       <c r="B79" s="3">
@@ -11314,7 +11313,7 @@
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A80">
+      <c r="A80" s="14">
         <v>195298</v>
       </c>
       <c r="B80" s="3">
@@ -11328,7 +11327,7 @@
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A81">
+      <c r="A81" s="14">
         <v>195998</v>
       </c>
       <c r="B81" s="3">
@@ -11339,7 +11338,7 @@
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A82">
+      <c r="A82" s="14">
         <v>196422</v>
       </c>
       <c r="B82" s="3">
@@ -11350,7 +11349,7 @@
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A83">
+      <c r="A83" s="14">
         <v>196425</v>
       </c>
       <c r="B83" s="3">
@@ -11361,7 +11360,7 @@
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A84">
+      <c r="A84" s="14">
         <v>196594</v>
       </c>
       <c r="B84" s="3">
@@ -11372,7 +11371,7 @@
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A85">
+      <c r="A85" s="14">
         <v>195849</v>
       </c>
       <c r="B85" s="3">
@@ -11383,7 +11382,7 @@
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A86">
+      <c r="A86" s="14">
         <v>196366</v>
       </c>
       <c r="B86" s="3">
@@ -11394,7 +11393,7 @@
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A87">
+      <c r="A87" s="14">
         <v>196372</v>
       </c>
       <c r="B87" s="3">
@@ -11405,7 +11404,7 @@
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A88">
+      <c r="A88" s="14">
         <v>196833</v>
       </c>
       <c r="B88" s="3">
@@ -11416,7 +11415,7 @@
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A89">
+      <c r="A89" s="14">
         <v>196834</v>
       </c>
       <c r="B89" s="3">
@@ -11427,7 +11426,7 @@
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A90">
+      <c r="A90" s="14">
         <v>196835</v>
       </c>
       <c r="B90" s="3">
@@ -11438,7 +11437,7 @@
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A91">
+      <c r="A91" s="14">
         <v>196675</v>
       </c>
       <c r="B91" s="3">
@@ -11449,7 +11448,7 @@
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A92">
+      <c r="A92" s="14">
         <v>196872</v>
       </c>
       <c r="B92" s="3">
@@ -11463,7 +11462,7 @@
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A93">
+      <c r="A93" s="14">
         <v>196424</v>
       </c>
       <c r="B93" s="3">
@@ -11474,7 +11473,7 @@
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A94">
+      <c r="A94" s="14">
         <v>196719</v>
       </c>
       <c r="B94" s="3">
@@ -11485,7 +11484,7 @@
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A95">
+      <c r="A95" s="14">
         <v>197199</v>
       </c>
       <c r="B95" s="3">
@@ -11496,7 +11495,7 @@
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A96">
+      <c r="A96" s="14">
         <v>197313</v>
       </c>
       <c r="B96" s="3">
@@ -11507,7 +11506,7 @@
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A97">
+      <c r="A97" s="14">
         <v>196429</v>
       </c>
       <c r="B97" s="3">
@@ -11518,7 +11517,7 @@
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A98">
+      <c r="A98" s="14">
         <v>196872</v>
       </c>
       <c r="B98" s="3">
@@ -11532,7 +11531,7 @@
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A99">
+      <c r="A99" s="14">
         <v>192992</v>
       </c>
       <c r="B99" s="3">
@@ -11560,16 +11559,17 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
+    <col min="1" max="1" width="9" style="14"/>
     <col min="2" max="3" width="10.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="13" t="s">
         <v>19</v>
       </c>
       <c r="B1" s="2" t="s">
@@ -11583,7 +11583,7 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A2">
+      <c r="A2" s="14">
         <v>197745</v>
       </c>
       <c r="B2" s="3">
@@ -11592,7 +11592,7 @@
       <c r="C2" s="3"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A3">
+      <c r="A3" s="14">
         <v>197757</v>
       </c>
       <c r="B3" s="3">
@@ -11601,7 +11601,7 @@
       <c r="C3" s="3"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A4">
+      <c r="A4" s="14">
         <v>196650</v>
       </c>
       <c r="B4" s="3">
@@ -11619,17 +11619,18 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:XFD6"/>
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
+    <col min="1" max="1" width="9" style="14"/>
     <col min="2" max="2" width="10.5" customWidth="1"/>
     <col min="3" max="3" width="10.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="13" t="s">
         <v>19</v>
       </c>
       <c r="B1" s="2" t="s">
@@ -11643,7 +11644,7 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A2">
+      <c r="A2" s="14">
         <v>197721</v>
       </c>
       <c r="B2" s="3">
@@ -11657,7 +11658,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A3">
+      <c r="A3" s="14">
         <v>197623</v>
       </c>
       <c r="B3" s="3">
@@ -11668,7 +11669,7 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A4">
+      <c r="A4" s="14">
         <v>197634</v>
       </c>
       <c r="B4" s="3">
@@ -11679,7 +11680,7 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A5">
+      <c r="A5" s="14">
         <v>197699</v>
       </c>
       <c r="B5" s="3">
@@ -11690,7 +11691,7 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A6">
+      <c r="A6" s="14">
         <v>197908</v>
       </c>
       <c r="B6" s="3">

</xml_diff>